<commit_message>
fixing weightfactor, documentation update
</commit_message>
<xml_diff>
--- a/Documentation/R Microsim Model - Derived Data Dictionary.xlsx
+++ b/Documentation/R Microsim Model - Derived Data Dictionary.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="331">
   <si>
     <t>id</t>
   </si>
@@ -991,6 +994,27 @@
   </si>
   <si>
     <t>Float</t>
+  </si>
+  <si>
+    <t>taker</t>
+  </si>
+  <si>
+    <t>needer</t>
+  </si>
+  <si>
+    <t>anypay</t>
+  </si>
+  <si>
+    <t>Indicator for taking leave of any kind</t>
+  </si>
+  <si>
+    <t>Indicator for needing leave of any kind</t>
+  </si>
+  <si>
+    <t>Indicator for receiving any pay from employer while on leave</t>
+  </si>
+  <si>
+    <t>Column1</t>
   </si>
 </sst>
 </file>
@@ -1032,7 +1056,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1045,16 +1073,38 @@
 </styleSheet>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet2"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:F154" totalsRowShown="0">
-  <autoFilter ref="A1:F154"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:G157" totalsRowShown="0">
+  <autoFilter ref="A1:G157">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="0"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <tableColumns count="7">
     <tableColumn id="1" name="Variable Name"/>
     <tableColumn id="2" name="Variable Type"/>
     <tableColumn id="3" name="Variable Label"/>
     <tableColumn id="4" name="Valid Values"/>
     <tableColumn id="5" name="Value Label"/>
     <tableColumn id="6" name="Notes"/>
+    <tableColumn id="7" name="Column1" dataDxfId="0">
+      <calculatedColumnFormula>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1323,10 +1373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F154"/>
+  <dimension ref="A1:G157"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A123" sqref="A123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1339,7 +1389,7 @@
     <col min="6" max="6" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>141</v>
       </c>
@@ -1358,8 +1408,11 @@
       <c r="F1" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1372,8 +1425,12 @@
       <c r="D2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1389,8 +1446,12 @@
       <c r="F3" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1406,8 +1467,12 @@
       <c r="F4" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1423,8 +1488,12 @@
       <c r="F5" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1440,8 +1509,12 @@
       <c r="F6" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1457,8 +1530,12 @@
       <c r="F7" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1474,8 +1551,12 @@
       <c r="F8" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1491,8 +1572,12 @@
       <c r="F9" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1508,8 +1593,12 @@
       <c r="F10" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1525,8 +1614,12 @@
       <c r="F11" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1542,8 +1635,12 @@
       <c r="F12" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1559,8 +1656,12 @@
       <c r="F13" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1576,8 +1677,12 @@
       <c r="F14" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1590,8 +1695,12 @@
       <c r="D15" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1607,8 +1716,12 @@
       <c r="F16" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1624,8 +1737,12 @@
       <c r="E17" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1641,8 +1758,12 @@
       <c r="E18" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1655,8 +1776,12 @@
       <c r="D19" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1669,8 +1794,12 @@
       <c r="D20" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1683,8 +1812,12 @@
       <c r="D21" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1700,8 +1833,12 @@
       <c r="E22" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1717,8 +1854,12 @@
       <c r="E23" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1734,8 +1875,12 @@
       <c r="E24" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1751,8 +1896,12 @@
       <c r="E25" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1765,8 +1914,12 @@
       <c r="D26" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1779,8 +1932,12 @@
       <c r="D27" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1796,8 +1953,12 @@
       <c r="E28" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1813,8 +1974,12 @@
       <c r="E29" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1830,8 +1995,12 @@
       <c r="E30" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1847,8 +2016,12 @@
       <c r="E31" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1864,8 +2037,12 @@
       <c r="E32" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1881,8 +2058,12 @@
       <c r="E33" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G33">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1898,8 +2079,12 @@
       <c r="E34" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1912,8 +2097,12 @@
       <c r="D35" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G35">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1929,8 +2118,12 @@
       <c r="E36" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1946,8 +2139,12 @@
       <c r="E37" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G37">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1963,8 +2160,12 @@
       <c r="E38" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G38">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1980,8 +2181,12 @@
       <c r="E39" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G39">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1997,8 +2202,12 @@
       <c r="E40" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G40">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -2014,8 +2223,12 @@
       <c r="E41" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G41">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -2031,8 +2244,12 @@
       <c r="E42" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G42">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2048,8 +2265,12 @@
       <c r="E43" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G43">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2065,8 +2286,12 @@
       <c r="E44" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G44">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2082,8 +2307,12 @@
       <c r="E45" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G45">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -2099,8 +2328,12 @@
       <c r="E46" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G46">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -2116,8 +2349,12 @@
       <c r="E47" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G47">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -2133,8 +2370,12 @@
       <c r="E48" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G48">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -2150,8 +2391,12 @@
       <c r="E49" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G49">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -2167,8 +2412,12 @@
       <c r="E50" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G50">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -2184,8 +2433,12 @@
       <c r="E51" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G51">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -2201,8 +2454,12 @@
       <c r="E52" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G52">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -2218,8 +2475,12 @@
       <c r="E53" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G53">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -2235,8 +2496,12 @@
       <c r="E54" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G54">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -2252,8 +2517,12 @@
       <c r="E55" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G55">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -2269,8 +2538,12 @@
       <c r="E56" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G56">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -2286,8 +2559,12 @@
       <c r="E57" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G57">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -2303,8 +2580,12 @@
       <c r="E58" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G58">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -2320,8 +2601,12 @@
       <c r="E59" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G59">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -2337,8 +2622,12 @@
       <c r="E60" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G60">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -2354,8 +2643,12 @@
       <c r="E61" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G61">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -2371,8 +2664,12 @@
       <c r="E62" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G62">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -2388,8 +2685,12 @@
       <c r="E63" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G63">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -2405,8 +2706,12 @@
       <c r="E64" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G64">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -2422,8 +2727,12 @@
       <c r="E65" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G65">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -2439,8 +2748,12 @@
       <c r="E66" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G66">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -2456,8 +2769,12 @@
       <c r="E67" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G67">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -2473,8 +2790,12 @@
       <c r="E68" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G68">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -2487,8 +2808,12 @@
       <c r="D69" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G69">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -2501,8 +2826,12 @@
       <c r="D70" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G70">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>178</v>
       </c>
@@ -2518,8 +2847,12 @@
       <c r="F71" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G71">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -2535,8 +2868,12 @@
       <c r="E72" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G72">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>71</v>
       </c>
@@ -2549,8 +2886,12 @@
       <c r="D73" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G73">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -2563,8 +2904,12 @@
       <c r="D74" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G74">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>73</v>
       </c>
@@ -2580,8 +2925,12 @@
       <c r="E75" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G75">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>74</v>
       </c>
@@ -2597,8 +2946,12 @@
       <c r="E76" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G76">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>75</v>
       </c>
@@ -2614,8 +2967,12 @@
       <c r="F77" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G77">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>76</v>
       </c>
@@ -2631,8 +2988,12 @@
       <c r="E78" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G78">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>77</v>
       </c>
@@ -2648,24 +3009,36 @@
       <c r="E79" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G79">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D80">
         <v>2</v>
       </c>
       <c r="E80" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G80">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D81">
         <v>3</v>
       </c>
       <c r="E81" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G81">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>78</v>
       </c>
@@ -2681,24 +3054,36 @@
       <c r="E82" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G82">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D83">
         <v>2</v>
       </c>
       <c r="E83" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G83">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D84">
         <v>3</v>
       </c>
       <c r="E84" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G84">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>79</v>
       </c>
@@ -2711,8 +3096,12 @@
       <c r="D85" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G85">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>80</v>
       </c>
@@ -2728,8 +3117,12 @@
       <c r="E86" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G86">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>181</v>
       </c>
@@ -2742,8 +3135,12 @@
       <c r="D87" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G87">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>182</v>
       </c>
@@ -2756,8 +3153,12 @@
       <c r="D88" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G88">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>81</v>
       </c>
@@ -2776,8 +3177,12 @@
       <c r="F89" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G89">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>82</v>
       </c>
@@ -2796,8 +3201,12 @@
       <c r="F90" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G90">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>83</v>
       </c>
@@ -2816,8 +3225,12 @@
       <c r="F91" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G91">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>84</v>
       </c>
@@ -2836,8 +3249,12 @@
       <c r="F92" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G92">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>85</v>
       </c>
@@ -2856,8 +3273,12 @@
       <c r="F93" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G93">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>86</v>
       </c>
@@ -2876,8 +3297,12 @@
       <c r="F94" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G94">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>87</v>
       </c>
@@ -2896,8 +3321,12 @@
       <c r="F95" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G95">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>88</v>
       </c>
@@ -2916,8 +3345,12 @@
       <c r="F96" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G96">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>89</v>
       </c>
@@ -2936,8 +3369,12 @@
       <c r="F97" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G97">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>90</v>
       </c>
@@ -2956,8 +3393,12 @@
       <c r="F98" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G98">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>91</v>
       </c>
@@ -2976,8 +3417,12 @@
       <c r="F99" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G99">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>92</v>
       </c>
@@ -2996,8 +3441,12 @@
       <c r="F100" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G100">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>94</v>
       </c>
@@ -3016,8 +3465,12 @@
       <c r="F101" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G101">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>95</v>
       </c>
@@ -3033,8 +3486,12 @@
       <c r="E102" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G102">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>93</v>
       </c>
@@ -3047,8 +3504,12 @@
       <c r="D103" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G103">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>96</v>
       </c>
@@ -3064,40 +3525,60 @@
       <c r="E104" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G104">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D105" t="s">
         <v>307</v>
       </c>
       <c r="E105" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G105">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D106" t="s">
         <v>308</v>
       </c>
       <c r="E106" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G106">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D107" t="s">
         <v>309</v>
       </c>
       <c r="E107" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G107">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D108" t="s">
         <v>310</v>
       </c>
       <c r="E108" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G108">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>97</v>
       </c>
@@ -3113,8 +3594,12 @@
       <c r="F109" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G109">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>98</v>
       </c>
@@ -3130,8 +3615,12 @@
       <c r="F110" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G110">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>99</v>
       </c>
@@ -3144,8 +3633,12 @@
       <c r="D111" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G111">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>100</v>
       </c>
@@ -3161,8 +3654,12 @@
       <c r="E112" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G112">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>101</v>
       </c>
@@ -3175,8 +3672,12 @@
       <c r="D113" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G113">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>102</v>
       </c>
@@ -3195,8 +3696,12 @@
       <c r="F114" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G114">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>103</v>
       </c>
@@ -3212,8 +3717,12 @@
       <c r="F115" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G115">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>104</v>
       </c>
@@ -3229,8 +3738,12 @@
       <c r="F116" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G116">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>105</v>
       </c>
@@ -3246,8 +3759,12 @@
       <c r="F117" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G117">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>106</v>
       </c>
@@ -3263,8 +3780,12 @@
       <c r="F118" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G118">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>107</v>
       </c>
@@ -3280,8 +3801,12 @@
       <c r="F119" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G119">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>108</v>
       </c>
@@ -3297,8 +3822,12 @@
       <c r="F120" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G120">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>109</v>
       </c>
@@ -3317,8 +3846,12 @@
       <c r="F121" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G121">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>1</v>
       </c>
@@ -3337,8 +3870,12 @@
       <c r="F122" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G122">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>110</v>
       </c>
@@ -3357,8 +3894,12 @@
       <c r="F123" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G123">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>111</v>
       </c>
@@ -3374,8 +3915,12 @@
       <c r="F124" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G124">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>112</v>
       </c>
@@ -3391,8 +3936,12 @@
       <c r="F125" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G125">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>113</v>
       </c>
@@ -3408,8 +3957,12 @@
       <c r="F126" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G126">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>114</v>
       </c>
@@ -3425,8 +3978,12 @@
       <c r="F127" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G127">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>115</v>
       </c>
@@ -3442,8 +3999,12 @@
       <c r="F128" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G128">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>116</v>
       </c>
@@ -3459,8 +4020,12 @@
       <c r="F129" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G129">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>117</v>
       </c>
@@ -3476,8 +4041,12 @@
       <c r="F130" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G130">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>118</v>
       </c>
@@ -3493,8 +4062,12 @@
       <c r="F131" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G131">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>119</v>
       </c>
@@ -3510,8 +4083,12 @@
       <c r="F132" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G132">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>120</v>
       </c>
@@ -3527,8 +4104,12 @@
       <c r="F133" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G133">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>121</v>
       </c>
@@ -3544,8 +4125,12 @@
       <c r="F134" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G134">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>122</v>
       </c>
@@ -3561,8 +4146,12 @@
       <c r="F135" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G135">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>123</v>
       </c>
@@ -3578,8 +4167,12 @@
       <c r="F136" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G136">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>124</v>
       </c>
@@ -3598,8 +4191,12 @@
       <c r="F137" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G137">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>183</v>
       </c>
@@ -3618,8 +4215,12 @@
       <c r="F138" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G138">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>125</v>
       </c>
@@ -3638,8 +4239,12 @@
       <c r="F139" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G139">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>126</v>
       </c>
@@ -3658,8 +4263,12 @@
       <c r="F140" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G140">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>127</v>
       </c>
@@ -3675,8 +4284,12 @@
       <c r="F141" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G141">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>128</v>
       </c>
@@ -3692,8 +4305,12 @@
       <c r="F142" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G142">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>129</v>
       </c>
@@ -3709,8 +4326,12 @@
       <c r="F143" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G143">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>130</v>
       </c>
@@ -3729,8 +4350,12 @@
       <c r="F144" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G144">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>131</v>
       </c>
@@ -3746,8 +4371,12 @@
       <c r="F145" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G145">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>132</v>
       </c>
@@ -3766,8 +4395,12 @@
       <c r="F146" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G146">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>133</v>
       </c>
@@ -3783,8 +4416,12 @@
       <c r="F147" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G147">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>134</v>
       </c>
@@ -3803,8 +4440,12 @@
       <c r="F148" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G148">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>135</v>
       </c>
@@ -3820,8 +4461,12 @@
       <c r="F149" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G149">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>136</v>
       </c>
@@ -3840,8 +4485,12 @@
       <c r="F150" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G150">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>137</v>
       </c>
@@ -3857,8 +4506,12 @@
       <c r="F151" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G151">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>138</v>
       </c>
@@ -3877,8 +4530,12 @@
       <c r="F152" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G152">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>139</v>
       </c>
@@ -3894,8 +4551,12 @@
       <c r="F153" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G153">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>140</v>
       </c>
@@ -3913,6 +4574,82 @@
       </c>
       <c r="F154" t="s">
         <v>302</v>
+      </c>
+      <c r="G154">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>324</v>
+      </c>
+      <c r="B155" t="s">
+        <v>323</v>
+      </c>
+      <c r="C155" t="s">
+        <v>327</v>
+      </c>
+      <c r="D155" t="s">
+        <v>293</v>
+      </c>
+      <c r="E155" t="s">
+        <v>294</v>
+      </c>
+      <c r="F155" t="s">
+        <v>302</v>
+      </c>
+      <c r="G155">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>325</v>
+      </c>
+      <c r="B156" t="s">
+        <v>323</v>
+      </c>
+      <c r="C156" t="s">
+        <v>328</v>
+      </c>
+      <c r="D156" t="s">
+        <v>293</v>
+      </c>
+      <c r="E156" t="s">
+        <v>294</v>
+      </c>
+      <c r="F156" t="s">
+        <v>302</v>
+      </c>
+      <c r="G156">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>326</v>
+      </c>
+      <c r="B157" t="s">
+        <v>323</v>
+      </c>
+      <c r="C157" t="s">
+        <v>329</v>
+      </c>
+      <c r="D157" t="s">
+        <v>293</v>
+      </c>
+      <c r="E157" t="s">
+        <v>294</v>
+      </c>
+      <c r="F157" t="s">
+        <v>302</v>
+      </c>
+      <c r="G157">
+        <f>COUNTIF([1]!Table3[Python Variable Name],Table2[[#This Row],[Variable Name]])</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>